<commit_message>
Re-fit primary growth model
Refitted primary growth model after spotting three outliers in master data
</commit_message>
<xml_diff>
--- a/OutputFiles/Percent prediction.xlsx
+++ b/OutputFiles/Percent prediction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sujun\Documents\GitHub\Bacillus-cereus-exposure-assessment-model\OutputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2593AD02-08D9-4473-966E-824059C5694A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC11E09-A4E2-4672-AD72-850861D6C8F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{82664678-6B70-4CF0-A080-A0B768C667B4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{82664678-6B70-4CF0-A080-A0B768C667B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t xml:space="preserve">isolate </t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>d35(&gt;3 log)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isolate </t>
   </si>
 </sst>
 </file>
@@ -411,7 +414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7128FC8F-FF1D-45BE-B6EE-E35692101C96}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -554,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2755BFD0-68E1-44B1-A6AA-68EF68234E3F}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -568,7 +571,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>

</xml_diff>